<commit_message>
CSS00013 is nolonger required
</commit_message>
<xml_diff>
--- a/src/test/resources/batch/ighv-intakemanifest.xlsx
+++ b/src/test/resources/batch/ighv-intakemanifest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsoehalim/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsoehalim/eclipse-workspace/cora/src/test/resources/batch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44967D31-DBEF-BF4F-A36B-4CBF6BF82622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E81F915-7B6C-B84A-AE79-547EA870C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="203">
   <si>
     <t>Cora INTAKE manifest</t>
   </si>
@@ -665,27 +665,6 @@
   </si>
   <si>
     <t>SAMPLE_NAME5</t>
-  </si>
-  <si>
-    <t>Box2</t>
-  </si>
-  <si>
-    <t>A:6</t>
-  </si>
-  <si>
-    <t>Container6</t>
-  </si>
-  <si>
-    <t>SAMPLE_NAME6</t>
-  </si>
-  <si>
-    <t>unique6</t>
-  </si>
-  <si>
-    <t>subjectCode6</t>
-  </si>
-  <si>
-    <t>test6</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG15"/>
+  <dimension ref="A1:BG14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AS22" sqref="AS22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2740,219 +2719,76 @@
       </c>
       <c r="BG11" s="10"/>
     </row>
-    <row r="12" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="54">
-        <v>44644</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="U12" s="25"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="55"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="55">
-        <v>101.1</v>
-      </c>
-      <c r="AD12" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="AE12" s="54">
-        <v>44181</v>
-      </c>
-      <c r="AF12" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="AI12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AO12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AP12" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="AQ12" s="56">
-        <v>76</v>
-      </c>
-      <c r="AR12" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AT12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AU12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AV12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AW12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AX12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AY12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AZ12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BB12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BC12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BD12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BE12" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="BF12" s="25" t="s">
-        <v>178</v>
-      </c>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="40"/>
+      <c r="AR12" s="40"/>
+      <c r="AS12" s="40"/>
+      <c r="AT12" s="40"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="20"/>
+      <c r="AW12" s="20"/>
+      <c r="AX12" s="20"/>
+      <c r="AY12" s="20"/>
+      <c r="AZ12" s="40"/>
+      <c r="BA12" s="40"/>
+      <c r="BB12" s="40"/>
+      <c r="BC12" s="40"/>
+      <c r="BD12" s="40"/>
+      <c r="BE12" s="40"/>
+      <c r="BF12" s="40"/>
       <c r="BG12" s="10"/>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="20"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="20"/>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="20"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
-      <c r="AL13" s="20"/>
-      <c r="AM13" s="20"/>
-      <c r="AN13" s="20"/>
-      <c r="AO13" s="20"/>
-      <c r="AP13" s="20"/>
-      <c r="AQ13" s="40"/>
-      <c r="AR13" s="40"/>
-      <c r="AS13" s="40"/>
-      <c r="AT13" s="40"/>
-      <c r="AU13" s="20"/>
-      <c r="AV13" s="20"/>
-      <c r="AW13" s="20"/>
-      <c r="AX13" s="20"/>
-      <c r="AY13" s="20"/>
-      <c r="AZ13" s="40"/>
-      <c r="BA13" s="40"/>
-      <c r="BB13" s="40"/>
-      <c r="BC13" s="40"/>
-      <c r="BD13" s="40"/>
-      <c r="BE13" s="40"/>
-      <c r="BF13" s="40"/>
-      <c r="BG13" s="10"/>
+      <c r="A13" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2966,16 +2802,16 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>HoldingContainerType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>ContainerType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G12" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1 xml:space="preserve"> SpecimenType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H12" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1 xml:space="preserve"> SpecimenSource</formula1>
     </dataValidation>
   </dataValidations>
@@ -3405,23 +3241,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <URL xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </URL>
-    <_dlc_DocId xmlns="a134e188-d237-415e-9089-632cc8d2b4a8">ADAPTIVE-1653259474-6349</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="a134e188-d237-415e-9089-632cc8d2b4a8">
-      <Url>https://adaptivebio.sharepoint.com/engineering/_layouts/15/DocIdRedir.aspx?ID=ADAPTIVE-1653259474-6349</Url>
-      <Description>ADAPTIVE-1653259474-6349</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009574B466B7C21C4B9D80A860A3E13C1A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd793596002196d52fa40f8a6c8ea08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="87ba4a14-7e41-41c7-9f63-fc9ba18728c1" xmlns:ns3="a134e188-d237-415e-9089-632cc8d2b4a8" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e864093dbf6fe24f04cb571f9b23010" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3648,85 +3526,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <URL xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </URL>
+    <_dlc_DocId xmlns="a134e188-d237-415e-9089-632cc8d2b4a8">ADAPTIVE-1653259474-6349</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="a134e188-d237-415e-9089-632cc8d2b4a8">
+      <Url>https://adaptivebio.sharepoint.com/engineering/_layouts/15/DocIdRedir.aspx?ID=ADAPTIVE-1653259474-6349</Url>
+      <Description>ADAPTIVE-1653259474-6349</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FF37FDE-501D-48DC-9178-AA6A40941737}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a134e188-d237-415e-9089-632cc8d2b4a8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="87ba4a14-7e41-41c7-9f63-fc9ba18728c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030AB9D0-3CD7-41B6-9BD1-2380E994F20B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3747,18 +3580,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FF37FDE-501D-48DC-9178-AA6A40941737}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a134e188-d237-415e-9089-632cc8d2b4a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="87ba4a14-7e41-41c7-9f63-fc9ba18728c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding test for SR-9373:R4, R7
</commit_message>
<xml_diff>
--- a/src/test/resources/batch/ighv-intakemanifest.xlsx
+++ b/src/test/resources/batch/ighv-intakemanifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsoehalim/eclipse-workspace/cora/src/test/resources/batch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsoehalim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E81F915-7B6C-B84A-AE79-547EA870C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF64FD-231B-AD4B-AE26-E5E13BAE57D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34460" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cora Intake Manifest" sheetId="1" r:id="rId1"/>
@@ -586,70 +586,70 @@
     <t>Container4</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>EDTA</t>
+  </si>
+  <si>
+    <t>test notes</t>
+  </si>
+  <si>
+    <t>unique1</t>
+  </si>
+  <si>
+    <t>unique2</t>
+  </si>
+  <si>
+    <t>unique3</t>
+  </si>
+  <si>
+    <t>unique4</t>
+  </si>
+  <si>
+    <t>subjectCode1</t>
+  </si>
+  <si>
+    <t>subjectCode2</t>
+  </si>
+  <si>
+    <t>subjectCode3</t>
+  </si>
+  <si>
+    <t>subjectCode4</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
     <t>A:5</t>
   </si>
   <si>
     <t>Container5</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
+    <t>unique5</t>
+  </si>
+  <si>
+    <t>subjectCode5</t>
   </si>
   <si>
     <t>test5</t>
-  </si>
-  <si>
-    <t>EDTA</t>
-  </si>
-  <si>
-    <t>test notes</t>
-  </si>
-  <si>
-    <t>unique1</t>
-  </si>
-  <si>
-    <t>unique2</t>
-  </si>
-  <si>
-    <t>unique3</t>
-  </si>
-  <si>
-    <t>unique4</t>
-  </si>
-  <si>
-    <t>unique5</t>
-  </si>
-  <si>
-    <t>subjectCode1</t>
-  </si>
-  <si>
-    <t>subjectCode2</t>
-  </si>
-  <si>
-    <t>subjectCode3</t>
-  </si>
-  <si>
-    <t>subjectCode4</t>
-  </si>
-  <si>
-    <t>subjectCode5</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
   </si>
   <si>
     <t>SAMPLE_NAME1</t>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AL25" sqref="AL25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2022,10 +2022,10 @@
         <v>167</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>198</v>
@@ -2035,7 +2035,7 @@
         <v>44643</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>32</v>
@@ -2047,7 +2047,7 @@
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
       <c r="T7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U7" s="25"/>
       <c r="V7" s="55"/>
@@ -2061,89 +2061,89 @@
         <v>100.1</v>
       </c>
       <c r="AD7" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE7" s="54">
         <v>44180</v>
       </c>
       <c r="AF7" s="25" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AG7" s="25"/>
       <c r="AH7" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AI7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AK7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AL7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AN7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AO7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AP7" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AQ7" s="56">
         <v>75</v>
       </c>
       <c r="AR7" s="25" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AS7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AT7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AV7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AX7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BB7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BD7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF7" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG7" s="10"/>
     </row>
@@ -2165,10 +2165,10 @@
         <v>171</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>199</v>
@@ -2178,7 +2178,7 @@
         <v>44643</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M8" s="25" t="s">
         <v>32</v>
@@ -2190,7 +2190,7 @@
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U8" s="25"/>
       <c r="V8" s="55"/>
@@ -2204,89 +2204,89 @@
         <v>100.1</v>
       </c>
       <c r="AD8" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE8" s="54">
         <v>44180</v>
       </c>
       <c r="AF8" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AG8" s="25"/>
       <c r="AH8" s="25" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="AI8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AM8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AN8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AO8" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP8" s="25" t="s">
         <v>178</v>
-      </c>
-      <c r="AJ8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AK8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AO8" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="AP8" s="25" t="s">
-        <v>180</v>
       </c>
       <c r="AQ8" s="56">
         <v>75</v>
       </c>
       <c r="AR8" s="25" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AS8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AT8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AV8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AX8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BB8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BD8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF8" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG8" s="10"/>
     </row>
@@ -2308,10 +2308,10 @@
         <v>173</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>200</v>
@@ -2321,7 +2321,7 @@
         <v>44643</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M9" s="25" t="s">
         <v>32</v>
@@ -2333,7 +2333,7 @@
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
       <c r="T9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U9" s="25"/>
       <c r="V9" s="55"/>
@@ -2347,89 +2347,89 @@
         <v>100.1</v>
       </c>
       <c r="AD9" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE9" s="54">
         <v>44180</v>
       </c>
       <c r="AF9" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AG9" s="25"/>
       <c r="AH9" s="25" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AI9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AK9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AL9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AN9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AO9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AP9" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AQ9" s="56">
         <v>75</v>
       </c>
       <c r="AR9" s="25" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AS9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AT9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AV9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AX9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BB9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BD9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF9" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG9" s="10"/>
     </row>
@@ -2451,10 +2451,10 @@
         <v>175</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>201</v>
@@ -2464,7 +2464,7 @@
         <v>44643</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M10" s="25" t="s">
         <v>32</v>
@@ -2476,7 +2476,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U10" s="25"/>
       <c r="V10" s="55"/>
@@ -2490,89 +2490,89 @@
         <v>100.1</v>
       </c>
       <c r="AD10" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE10" s="54">
         <v>44180</v>
       </c>
       <c r="AF10" s="25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AG10" s="25"/>
       <c r="AH10" s="25" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AI10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AK10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AL10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AN10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AO10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AP10" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AQ10" s="56">
         <v>75</v>
       </c>
       <c r="AR10" s="25" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AS10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AT10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AV10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AX10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BB10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BD10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF10" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG10" s="10"/>
     </row>
@@ -2585,29 +2585,29 @@
         <v>168</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>202</v>
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="54">
-        <v>44643</v>
+        <v>44644</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M11" s="25" t="s">
         <v>32</v>
@@ -2619,7 +2619,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
       <c r="T11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U11" s="25"/>
       <c r="V11" s="55"/>
@@ -2630,92 +2630,92 @@
       <c r="AA11" s="25"/>
       <c r="AB11" s="25"/>
       <c r="AC11" s="55">
-        <v>100.1</v>
+        <v>101.1</v>
       </c>
       <c r="AD11" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE11" s="54">
-        <v>44180</v>
+        <v>44181</v>
       </c>
       <c r="AF11" s="25" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AG11" s="25"/>
       <c r="AH11" s="25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AI11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AK11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AL11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AN11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AO11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AP11" s="25" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="AQ11" s="56">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AR11" s="25" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AS11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AT11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AV11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AX11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AZ11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BB11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BD11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BF11" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG11" s="10"/>
     </row>
@@ -2808,10 +2808,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>ContainerType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G11" xr:uid="{7BDC2EA7-EF36-1043-8273-546CF98198B5}">
       <formula1 xml:space="preserve"> SpecimenType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H11" xr:uid="{020B08AB-44B2-8C4B-9D5D-3C19BB2F6D8E}">
       <formula1 xml:space="preserve"> SpecimenSource</formula1>
     </dataValidation>
   </dataValidations>
@@ -3241,65 +3241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009574B466B7C21C4B9D80A860A3E13C1A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd793596002196d52fa40f8a6c8ea08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="87ba4a14-7e41-41c7-9f63-fc9ba18728c1" xmlns:ns3="a134e188-d237-415e-9089-632cc8d2b4a8" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e864093dbf6fe24f04cb571f9b23010" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3526,6 +3467,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3544,22 +3544,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030AB9D0-3CD7-41B6-9BD1-2380E994F20B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3580,21 +3564,37 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FF37FDE-501D-48DC-9178-AA6A40941737}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="a134e188-d237-415e-9089-632cc8d2b4a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="87ba4a14-7e41-41c7-9f63-fc9ba18728c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>